<commit_message>
Version 1.4 Das Eigabe-Window mit dem QT-Designer erstellt
</commit_message>
<xml_diff>
--- a/sql_results.xlsx
+++ b/sql_results.xlsx
@@ -10,7 +10,7 @@
     <sheet name="SQL Ergebnisse" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SQL Ergebnisse'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'SQL Ergebnisse'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -437,7 +437,10 @@
     <col width="9" customWidth="1" min="1" max="1"/>
     <col width="5" customWidth="1" min="2" max="2"/>
     <col width="9" customWidth="1" min="3" max="3"/>
-    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="37" customWidth="1" min="6" max="6"/>
+    <col width="16" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -458,7 +461,22 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>00001</t>
+          <t>FSKONZ</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>FSFIRM</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>FSAN1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>BESTANDSMODULE</t>
         </is>
       </c>
     </row>
@@ -478,12 +496,447 @@
           <t>E09</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>18</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>D01</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>040</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>                                   </t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>S01</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>020</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Google Germany GmbH                </t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>D01</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>030</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Test F.Bäcker                      </t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>8686</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>D12</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Test AKL                           </t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>D97</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FIEGE Logistik Stiftung &amp; Co. KG   </t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>S01</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>SME</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sascha Mergard                     </t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>D14</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">JBE                                </t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>F01</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Firat Askin                        </t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>D80</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>FFA</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A                                  </t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>D02</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>010</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">.                                  </t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>D13</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>BWO</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bastian Woltemade GmbH             </t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>D99</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>000</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Schulung                           </t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HV9</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>TST</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>E09</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>D03</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KST TESTFIRMA                      </t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>